<commit_message>
Regenerate model results for Tony
</commit_message>
<xml_diff>
--- a/draft-02/manuscript_ver3-4/model-summary-for-Tony.xlsx
+++ b/draft-02/manuscript_ver3-4/model-summary-for-Tony.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruanvanmazijk/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruanvanmazijk/Desktop/Cape-vs-SWA/draft-02/manuscript_ver3-4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{634FA508-B2D3-454F-8D07-180AD22712F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231F0301-22DC-B940-AE01-E7374D980503}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="960" windowWidth="14620" windowHeight="16040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="model-summary-for-Tony" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="44">
   <si>
     <t>(Intercept)</t>
   </si>
@@ -143,6 +143,15 @@
   </si>
   <si>
     <t>.</t>
+  </si>
+  <si>
+    <t>(295.543)</t>
+  </si>
+  <si>
+    <t>(829.526)</t>
+  </si>
+  <si>
+    <t>(2783.539)</t>
   </si>
 </sst>
 </file>
@@ -622,16 +631,19 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -990,7 +1002,7 @@
   <dimension ref="A1:I48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1014,14 +1026,14 @@
       <c r="C1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="4"/>
       <c r="H1" s="2" t="s">
         <v>28</v>
       </c>
@@ -1047,8 +1059,8 @@
       <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="C4">
-        <v>295.54300000000001</v>
+      <c r="C4" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="D4">
         <v>255.28800000000001</v>
@@ -1376,8 +1388,8 @@
       <c r="B18" t="s">
         <v>0</v>
       </c>
-      <c r="C18">
-        <v>829.52599999999995</v>
+      <c r="C18" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="D18">
         <v>672.90700000000004</v>
@@ -1737,7 +1749,7 @@
       <c r="H32" s="1">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="I32" s="3" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1774,8 +1786,8 @@
       <c r="B35" t="s">
         <v>0</v>
       </c>
-      <c r="C35">
-        <v>2783.5390000000002</v>
+      <c r="C35" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="D35">
         <v>2136.19</v>
@@ -1870,7 +1882,7 @@
       <c r="H38" s="1">
         <v>2E-3</v>
       </c>
-      <c r="I38" s="4" t="s">
+      <c r="I38" s="3" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2095,7 +2107,7 @@
       <c r="H47" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="I47" s="4" t="s">
+      <c r="I47" s="3" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>